<commit_message>
Availability plot nice now
</commit_message>
<xml_diff>
--- a/Data/Sites_overview.xlsx
+++ b/Data/Sites_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Documents\GitHub\EU_Overview\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EF47C2-494E-446F-A801-B02A682457F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A92B1A-28AE-4569-B939-50F67A8FB467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1395" yWindow="3585" windowWidth="14745" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="312">
   <si>
     <t>Site</t>
   </si>
@@ -1023,6 +1023,12 @@
   </si>
   <si>
     <t>MSC</t>
+  </si>
+  <si>
+    <t>Madrid - CIEMAT</t>
+  </si>
+  <si>
+    <t>MAD</t>
   </si>
 </sst>
 </file>
@@ -1835,11 +1841,11 @@
     <xf numFmtId="0" fontId="0" fillId="41" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -2215,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X66"/>
+  <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
+      <selection sqref="A1:V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,10 +2367,10 @@
       <c r="S2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="66" t="s">
+      <c r="T2" s="65" t="s">
         <v>205</v>
       </c>
-      <c r="U2" s="66" t="s">
+      <c r="U2" s="65" t="s">
         <v>305</v>
       </c>
       <c r="V2" s="44" t="s">
@@ -2594,7 +2600,7 @@
       <c r="H6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="65">
+      <c r="I6" s="64">
         <v>40864</v>
       </c>
       <c r="J6" s="21">
@@ -2963,7 +2969,7 @@
     </row>
     <row r="12" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56">
-        <f>A11+1</f>
+        <f t="shared" ref="A12:A40" si="0">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -3028,7 +3034,7 @@
     </row>
     <row r="13" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3093,7 +3099,7 @@
     </row>
     <row r="14" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -3158,7 +3164,7 @@
     </row>
     <row r="15" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -3225,7 +3231,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="37">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3292,7 +3298,7 @@
     </row>
     <row r="17" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3357,7 +3363,7 @@
     </row>
     <row r="18" spans="1:22" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3422,7 +3428,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3489,7 +3495,7 @@
     </row>
     <row r="20" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3556,7 +3562,7 @@
     </row>
     <row r="21" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3621,7 +3627,7 @@
     </row>
     <row r="22" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3686,7 +3692,7 @@
     </row>
     <row r="23" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3751,44 +3757,43 @@
     </row>
     <row r="24" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f>A23+1</f>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>247</v>
+        <v>310</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>311</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="45">
-        <v>46.2</v>
-      </c>
-      <c r="F24" s="45">
-        <v>8.9</v>
-      </c>
-      <c r="G24" s="45">
-        <v>203</v>
+        <v>34</v>
+      </c>
+      <c r="E24" s="46">
+        <v>40.456435999999997</v>
+      </c>
+      <c r="F24" s="46">
+        <v>-3.7256309999999999</v>
+      </c>
+      <c r="G24" s="46">
+        <v>669</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="I24" s="21">
-        <v>41514</v>
+        <v>43729</v>
       </c>
       <c r="J24" s="21">
-        <v>41942</v>
+        <v>45291</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="18" t="s">
-        <v>7</v>
+      <c r="L24" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N24" s="53"/>
       <c r="O24" s="4" t="s">
@@ -3801,7 +3806,7 @@
         <v>15</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>168</v>
+        <v>36</v>
       </c>
       <c r="S24" s="4" t="s">
         <v>24</v>
@@ -3809,64 +3814,61 @@
       <c r="T24" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="U24" s="4" t="s">
-        <v>250</v>
-      </c>
+      <c r="U24" s="4"/>
       <c r="V24" s="18"/>
     </row>
     <row r="25" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37">
-        <f>A24+1</f>
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>252</v>
+        <v>69</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="46">
-        <v>53.44417</v>
-      </c>
-      <c r="F25" s="46">
-        <v>-2.2144439999999999</v>
-      </c>
-      <c r="G25" s="46">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="E25" s="45">
+        <v>46.2</v>
+      </c>
+      <c r="F25" s="45">
+        <v>8.9</v>
+      </c>
+      <c r="G25" s="45">
+        <v>203</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>213</v>
+        <v>248</v>
       </c>
       <c r="I25" s="21">
-        <v>43889</v>
+        <v>41514</v>
       </c>
       <c r="J25" s="21">
-        <v>45020</v>
+        <v>41942</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="55" t="s">
-        <v>8</v>
+      <c r="L25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="N25" s="53"/>
       <c r="O25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>214</v>
+        <v>12</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>215</v>
+        <v>15</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
       <c r="S25" s="4" t="s">
         <v>24</v>
@@ -3875,121 +3877,119 @@
         <v>205</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>296</v>
+        <v>250</v>
       </c>
       <c r="V25" s="18"/>
     </row>
     <row r="26" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <f>A25+1</f>
+      <c r="A26" s="37">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="45">
-        <v>43.305233000000001</v>
-      </c>
-      <c r="F26" s="45">
-        <v>5.394692</v>
-      </c>
-      <c r="G26" s="45">
-        <v>71</v>
+      <c r="E26" s="46">
+        <v>53.44417</v>
+      </c>
+      <c r="F26" s="46">
+        <v>-2.2144439999999999</v>
+      </c>
+      <c r="G26" s="46">
+        <v>43</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="I26" s="21">
-        <v>42947</v>
+        <v>43889</v>
       </c>
       <c r="J26" s="21">
-        <v>44925</v>
+        <v>45020</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="M26" s="18" t="s">
-        <v>7</v>
+      <c r="L26" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" s="55" t="s">
+        <v>8</v>
       </c>
       <c r="N26" s="53"/>
       <c r="O26" s="4" t="s">
-        <v>203</v>
+        <v>10</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>12</v>
+        <v>214</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>23</v>
+        <v>253</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>246</v>
+        <v>24</v>
       </c>
       <c r="T26" s="4" t="s">
         <v>205</v>
       </c>
       <c r="U26" s="4" t="s">
-        <v>256</v>
+        <v>296</v>
       </c>
       <c r="V26" s="18"/>
     </row>
     <row r="27" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62">
-        <f>A26+1</f>
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="45">
+        <v>43.305233000000001</v>
+      </c>
+      <c r="F27" s="45">
+        <v>5.394692</v>
+      </c>
+      <c r="G27" s="45">
         <v>71</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="45">
-        <v>51.54</v>
-      </c>
-      <c r="F27" s="45">
-        <v>12.93</v>
-      </c>
-      <c r="G27" s="45">
-        <v>86</v>
-      </c>
       <c r="H27" s="4" t="s">
-        <v>4</v>
+        <v>181</v>
       </c>
       <c r="I27" s="21">
-        <v>42621</v>
+        <v>42947</v>
       </c>
       <c r="J27" s="21">
-        <v>42978</v>
+        <v>44925</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L27" s="55" t="s">
-        <v>8</v>
+      <c r="L27" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="M27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="N27" s="53" t="s">
-        <v>8</v>
-      </c>
+      <c r="N27" s="53"/>
       <c r="O27" s="4" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
       <c r="P27" s="4" t="s">
         <v>12</v>
@@ -4001,47 +4001,47 @@
         <v>23</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>205</v>
       </c>
       <c r="U27" s="4" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="V27" s="18"/>
     </row>
     <row r="28" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37">
-        <f>A27+1</f>
+      <c r="A28" s="62">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>245</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E28" s="45">
-        <v>53.3</v>
+        <v>51.54</v>
       </c>
       <c r="F28" s="45">
-        <v>-9.9</v>
+        <v>12.93</v>
       </c>
       <c r="G28" s="45">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>220</v>
+        <v>4</v>
       </c>
       <c r="I28" s="21">
-        <v>42377</v>
+        <v>42621</v>
       </c>
       <c r="J28" s="21">
-        <v>43294</v>
+        <v>42978</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>7</v>
@@ -4049,12 +4049,14 @@
       <c r="L28" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="55" t="s">
+      <c r="M28" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="N28" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="N28" s="53"/>
       <c r="O28" s="4" t="s">
-        <v>287</v>
+        <v>10</v>
       </c>
       <c r="P28" s="4" t="s">
         <v>12</v>
@@ -4066,60 +4068,60 @@
         <v>23</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>205</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="V28" s="18"/>
     </row>
     <row r="29" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <f>A28+1</f>
+      <c r="A29" s="37">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>197</v>
+        <v>244</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>198</v>
+        <v>245</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E29" s="45">
-        <v>45.478611000000001</v>
+        <v>53.3</v>
       </c>
       <c r="F29" s="45">
-        <v>9.2344439999999999</v>
-      </c>
-      <c r="G29" s="46">
-        <v>118</v>
+        <v>-9.9</v>
+      </c>
+      <c r="G29" s="45">
+        <v>5</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>22</v>
+        <v>220</v>
       </c>
       <c r="I29" s="21">
-        <v>41673</v>
+        <v>42377</v>
       </c>
       <c r="J29" s="21">
-        <v>41698</v>
+        <v>43294</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N29" s="4"/>
+      <c r="L29" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="M29" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="N29" s="53"/>
       <c r="O29" s="4" t="s">
-        <v>41</v>
+        <v>287</v>
       </c>
       <c r="P29" s="4" t="s">
         <v>12</v>
@@ -4131,7 +4133,7 @@
         <v>23</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>17</v>
+        <v>246</v>
       </c>
       <c r="T29" s="4" t="s">
         <v>205</v>
@@ -4141,169 +4143,169 @@
       </c>
       <c r="V29" s="18"/>
     </row>
-    <row r="30" spans="1:22" s="33" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37">
-        <f>A29+1</f>
+    <row r="30" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>307</v>
+        <v>197</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="E30" s="46">
-        <v>42.05</v>
-      </c>
-      <c r="F30" s="46">
-        <v>0.72</v>
+        <v>198</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="45">
+        <v>45.478611000000001</v>
+      </c>
+      <c r="F30" s="45">
+        <v>9.2344439999999999</v>
       </c>
       <c r="G30" s="46">
-        <v>1570</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="I30" s="43">
-        <v>40738</v>
-      </c>
-      <c r="J30" s="43">
-        <v>41022</v>
-      </c>
-      <c r="K30" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="L30" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="M30" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="N30" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="O30" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="P30" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="21">
+        <v>41673</v>
+      </c>
+      <c r="J30" s="21">
+        <v>41698</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q30" s="18" t="s">
+      <c r="Q30" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R30" s="18" t="s">
+      <c r="R30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S30" s="18" t="s">
-        <v>291</v>
+      <c r="S30" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="T30" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="U30" s="18" t="s">
-        <v>308</v>
+      <c r="U30" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="V30" s="18"/>
     </row>
-    <row r="31" spans="1:22" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>A30+1</f>
+    <row r="31" spans="1:22" s="33" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="37">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>257</v>
+        <v>307</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>32</v>
+        <v>309</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="E31" s="46">
-        <v>41.779342</v>
+        <v>42.05</v>
       </c>
       <c r="F31" s="46">
-        <v>2.3580329999999998</v>
+        <v>0.72</v>
       </c>
       <c r="G31" s="46">
-        <v>720</v>
-      </c>
-      <c r="H31" s="4" t="s">
+        <v>1570</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="I31" s="21">
-        <v>44426</v>
-      </c>
-      <c r="J31" s="21">
-        <v>44711</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="55" t="s">
+      <c r="I31" s="43">
+        <v>40738</v>
+      </c>
+      <c r="J31" s="43">
+        <v>41022</v>
+      </c>
+      <c r="K31" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="18"/>
-      <c r="O31" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="P31" s="4" t="s">
+      <c r="M31" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="N31" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="O31" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P31" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="Q31" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="R31" s="4" t="s">
+      <c r="Q31" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R31" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="S31" s="4" t="s">
-        <v>246</v>
+      <c r="S31" s="18" t="s">
+        <v>291</v>
       </c>
       <c r="T31" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="U31" s="4" t="s">
-        <v>296</v>
+      <c r="U31" s="18" t="s">
+        <v>308</v>
       </c>
       <c r="V31" s="18"/>
     </row>
-    <row r="32" spans="1:22" s="33" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38">
-        <f>A31+1</f>
+    <row r="32" spans="1:22" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>207</v>
+        <v>257</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="50">
-        <v>37.973439999999997</v>
-      </c>
-      <c r="F32" s="50">
-        <v>23.718084999999999</v>
-      </c>
-      <c r="G32" s="50">
-        <v>105</v>
+        <v>77</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="46">
+        <v>41.779342</v>
+      </c>
+      <c r="F32" s="46">
+        <v>2.3580329999999998</v>
+      </c>
+      <c r="G32" s="46">
+        <v>720</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>157</v>
+        <v>229</v>
       </c>
       <c r="I32" s="21">
-        <v>42736</v>
+        <v>44426</v>
       </c>
       <c r="J32" s="21">
-        <v>44531</v>
+        <v>44711</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>7</v>
@@ -4316,19 +4318,19 @@
       </c>
       <c r="N32" s="18"/>
       <c r="O32" s="4" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
       <c r="P32" s="4" t="s">
         <v>12</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>15</v>
+        <v>258</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>23</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>24</v>
+        <v>246</v>
       </c>
       <c r="T32" s="4" t="s">
         <v>205</v>
@@ -4336,52 +4338,52 @@
       <c r="U32" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="V32" s="27"/>
-    </row>
-    <row r="33" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f>A32+1</f>
+      <c r="V32" s="18"/>
+    </row>
+    <row r="33" spans="1:24" s="33" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="38">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>207</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="51">
-        <v>45.377499999999998</v>
-      </c>
-      <c r="F33" s="51">
-        <v>11.94</v>
+      <c r="E33" s="50">
+        <v>37.973439999999997</v>
+      </c>
+      <c r="F33" s="50">
+        <v>23.718084999999999</v>
       </c>
       <c r="G33" s="50">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="I33" s="21">
-        <v>41665</v>
+        <v>42736</v>
       </c>
       <c r="J33" s="21">
-        <v>41698</v>
+        <v>44531</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L33" s="55" t="s">
+      <c r="L33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="M33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N33" s="4"/>
+      <c r="N33" s="18"/>
       <c r="O33" s="4" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="P33" s="4" t="s">
         <v>12</v>
@@ -4401,52 +4403,50 @@
       <c r="U33" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="V33" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" s="28" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38">
-        <f>A33+1</f>
+      <c r="V33" s="27"/>
+    </row>
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>260</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>261</v>
+        <v>40</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="45">
-        <v>50.1</v>
-      </c>
-      <c r="F34" s="45">
-        <v>14.4</v>
-      </c>
-      <c r="G34" s="45">
-        <v>277</v>
+      <c r="E34" s="51">
+        <v>45.377499999999998</v>
+      </c>
+      <c r="F34" s="51">
+        <v>11.94</v>
+      </c>
+      <c r="G34" s="50">
+        <v>11</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>262</v>
+        <v>22</v>
       </c>
       <c r="I34" s="21">
-        <v>41080</v>
+        <v>41665</v>
       </c>
       <c r="J34" s="21">
-        <v>41409</v>
+        <v>41698</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="55" t="s">
+      <c r="L34" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="N34" s="18"/>
+      <c r="M34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" s="4"/>
       <c r="O34" s="4" t="s">
         <v>41</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>15</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>168</v>
+        <v>23</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>24</v>
@@ -4466,54 +4466,56 @@
         <v>205</v>
       </c>
       <c r="U34" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="V34" s="4"/>
-    </row>
-    <row r="35" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="56">
-        <f>A34+1</f>
+        <v>296</v>
+      </c>
+      <c r="V34" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" s="28" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="38">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E35" s="50">
-        <v>45.766669999999998</v>
-      </c>
-      <c r="F35" s="50">
-        <v>2.95</v>
-      </c>
-      <c r="G35" s="50">
-        <v>1465</v>
+        <v>34</v>
+      </c>
+      <c r="E35" s="45">
+        <v>50.1</v>
+      </c>
+      <c r="F35" s="45">
+        <v>14.4</v>
+      </c>
+      <c r="G35" s="45">
+        <v>277</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>181</v>
+        <v>262</v>
       </c>
       <c r="I35" s="21">
-        <v>43622</v>
+        <v>41080</v>
       </c>
       <c r="J35" s="21">
-        <v>44195</v>
+        <v>41409</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L35" s="55" t="s">
-        <v>8</v>
+      <c r="L35" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="M35" s="55" t="s">
         <v>8</v>
       </c>
       <c r="N35" s="18"/>
       <c r="O35" s="4" t="s">
-        <v>203</v>
+        <v>41</v>
       </c>
       <c r="P35" s="4" t="s">
         <v>12</v>
@@ -4522,52 +4524,50 @@
         <v>15</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>23</v>
+        <v>168</v>
       </c>
       <c r="S35" s="4" t="s">
-        <v>216</v>
+        <v>24</v>
       </c>
       <c r="T35" s="4" t="s">
         <v>205</v>
       </c>
       <c r="U35" s="4" t="s">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="V35" s="4"/>
-      <c r="W35" s="7"/>
-      <c r="X35" s="6"/>
     </row>
     <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="61">
-        <f>A35+1</f>
+      <c r="A36" s="56">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>225</v>
+        <v>264</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>226</v>
+        <v>265</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E36" s="45">
-        <v>48.71</v>
-      </c>
-      <c r="F36" s="45">
-        <v>2.15</v>
-      </c>
-      <c r="G36" s="45">
-        <v>163</v>
+        <v>173</v>
+      </c>
+      <c r="E36" s="50">
+        <v>45.766669999999998</v>
+      </c>
+      <c r="F36" s="50">
+        <v>2.95</v>
+      </c>
+      <c r="G36" s="50">
+        <v>1465</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>181</v>
       </c>
       <c r="I36" s="21">
-        <v>40695</v>
+        <v>43622</v>
       </c>
       <c r="J36" s="21">
-        <v>44921</v>
+        <v>44195</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>7</v>
@@ -4578,9 +4578,9 @@
       <c r="M36" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="N36" s="53"/>
+      <c r="N36" s="18"/>
       <c r="O36" s="4" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
       <c r="P36" s="4" t="s">
         <v>12</v>
@@ -4592,183 +4592,183 @@
         <v>23</v>
       </c>
       <c r="S36" s="4" t="s">
-        <v>24</v>
+        <v>216</v>
       </c>
       <c r="T36" s="4" t="s">
         <v>205</v>
       </c>
       <c r="U36" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="V36" s="27"/>
+        <v>296</v>
+      </c>
+      <c r="V36" s="4"/>
       <c r="W36" s="7"/>
       <c r="X36" s="6"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <f>A36+1</f>
+      <c r="A37" s="61">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="46">
-        <v>61.8</v>
-      </c>
-      <c r="F37" s="46">
-        <v>24.3</v>
-      </c>
-      <c r="G37" s="46">
+      <c r="B37" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E37" s="45">
+        <v>48.71</v>
+      </c>
+      <c r="F37" s="45">
+        <v>2.15</v>
+      </c>
+      <c r="G37" s="45">
+        <v>163</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H37" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="I37" s="41">
-        <v>40908</v>
-      </c>
-      <c r="J37" s="41">
-        <v>44196</v>
-      </c>
-      <c r="K37" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="L37" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N37" s="54"/>
-      <c r="O37" s="41" t="s">
+      <c r="I37" s="21">
+        <v>40695</v>
+      </c>
+      <c r="J37" s="21">
+        <v>44921</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="M37" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="N37" s="53"/>
+      <c r="O37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P37" s="41" t="s">
+      <c r="P37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q37" s="41" t="s">
+      <c r="Q37" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R37" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="S37" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="T37" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="U37" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="V37" s="41"/>
+      <c r="R37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S37" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="V37" s="27"/>
       <c r="W37" s="7"/>
       <c r="X37" s="6"/>
     </row>
     <row r="38" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="56">
-        <f>A37+1</f>
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="B38" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="51">
-        <v>44.524444000000003</v>
-      </c>
-      <c r="F38" s="51">
-        <v>11.524444000000001</v>
-      </c>
-      <c r="G38" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I38" s="21">
-        <v>40861</v>
-      </c>
-      <c r="J38" s="21">
-        <v>42347</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L38" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P38" s="4" t="s">
+      <c r="E38" s="46">
+        <v>61.8</v>
+      </c>
+      <c r="F38" s="46">
+        <v>24.3</v>
+      </c>
+      <c r="G38" s="46">
+        <v>181</v>
+      </c>
+      <c r="H38" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="I38" s="41">
+        <v>40908</v>
+      </c>
+      <c r="J38" s="41">
+        <v>44196</v>
+      </c>
+      <c r="K38" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="N38" s="54"/>
+      <c r="O38" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="P38" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="Q38" s="4" t="s">
+      <c r="Q38" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="R38" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="S38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T38" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="U38" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="V38" s="4"/>
+      <c r="R38" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="S38" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="T38" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="U38" s="41" t="s">
+        <v>233</v>
+      </c>
+      <c r="V38" s="41"/>
       <c r="W38" s="7"/>
       <c r="X38" s="6"/>
     </row>
     <row r="39" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="56">
-        <f>A38+1</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="45">
-        <v>58.370600000000003</v>
-      </c>
-      <c r="F39" s="45">
-        <v>26.7349</v>
-      </c>
-      <c r="G39" s="45">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="E39" s="51">
+        <v>44.524444000000003</v>
+      </c>
+      <c r="F39" s="51">
+        <v>11.524444000000001</v>
+      </c>
+      <c r="G39" s="49" t="s">
+        <v>152</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>276</v>
+        <v>22</v>
       </c>
       <c r="I39" s="21">
-        <v>42614</v>
+        <v>40861</v>
       </c>
       <c r="J39" s="21">
-        <v>42940</v>
+        <v>42347</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>7</v>
@@ -4779,11 +4779,9 @@
       <c r="M39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N39" s="53" t="s">
-        <v>8</v>
-      </c>
+      <c r="N39" s="4"/>
       <c r="O39" s="4" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="P39" s="4" t="s">
         <v>12</v>
@@ -4792,51 +4790,52 @@
         <v>15</v>
       </c>
       <c r="R39" s="4" t="s">
-        <v>23</v>
+        <v>270</v>
       </c>
       <c r="S39" s="4" t="s">
-        <v>216</v>
+        <v>17</v>
       </c>
       <c r="T39" s="4" t="s">
         <v>205</v>
       </c>
       <c r="U39" s="4" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="V39" s="4"/>
       <c r="W39" s="7"/>
       <c r="X39" s="6"/>
     </row>
     <row r="40" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="37">
+      <c r="A40" s="56">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>87</v>
+        <v>273</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E40" s="45">
-        <v>60.5</v>
+        <v>58.370600000000003</v>
       </c>
       <c r="F40" s="45">
-        <v>27.7</v>
+        <v>26.7349</v>
       </c>
       <c r="G40" s="45">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>154</v>
+        <v>276</v>
       </c>
       <c r="I40" s="21">
-        <v>41075</v>
+        <v>42614</v>
       </c>
       <c r="J40" s="21">
-        <v>41432</v>
+        <v>42940</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>7</v>
@@ -4844,10 +4843,12 @@
       <c r="L40" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="M40" s="55" t="s">
+      <c r="M40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N40" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="N40" s="18"/>
       <c r="O40" s="4" t="s">
         <v>10</v>
       </c>
@@ -4858,10 +4859,10 @@
         <v>15</v>
       </c>
       <c r="R40" s="4" t="s">
-        <v>155</v>
+        <v>23</v>
       </c>
       <c r="S40" s="4" t="s">
-        <v>24</v>
+        <v>216</v>
       </c>
       <c r="T40" s="4" t="s">
         <v>205</v>
@@ -4873,37 +4874,36 @@
       <c r="W40" s="7"/>
       <c r="X40" s="6"/>
     </row>
-    <row r="41" spans="1:24" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="37">
-        <f>A40+1</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>293</v>
+        <v>87</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>294</v>
+        <v>32</v>
       </c>
       <c r="E41" s="45">
-        <v>78.907150000000001</v>
+        <v>60.5</v>
       </c>
       <c r="F41" s="45">
-        <v>-11.886799999999999</v>
+        <v>27.7</v>
       </c>
       <c r="G41" s="45">
-        <v>474</v>
+        <v>7</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>210</v>
+        <v>154</v>
       </c>
       <c r="I41" s="21">
-        <v>44562</v>
+        <v>41075</v>
       </c>
       <c r="J41" s="21">
-        <v>44910</v>
+        <v>41432</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>7</v>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="N41" s="18"/>
       <c r="O41" s="4" t="s">
-        <v>203</v>
+        <v>10</v>
       </c>
       <c r="P41" s="4" t="s">
         <v>12</v>
@@ -4925,10 +4925,10 @@
         <v>15</v>
       </c>
       <c r="R41" s="4" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="S41" s="4" t="s">
-        <v>291</v>
+        <v>24</v>
       </c>
       <c r="T41" s="4" t="s">
         <v>205</v>
@@ -4940,52 +4940,50 @@
       <c r="W41" s="7"/>
       <c r="X41" s="6"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <f>A41+1</f>
-        <v>41</v>
+    <row r="42" spans="1:24" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="37">
+        <f t="shared" ref="A42:A50" si="1">A41+1</f>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>89</v>
+        <v>293</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>34</v>
+        <v>294</v>
       </c>
       <c r="E42" s="45">
-        <v>47.4</v>
+        <v>78.907150000000001</v>
       </c>
       <c r="F42" s="45">
-        <v>8.5</v>
+        <v>-11.886799999999999</v>
       </c>
       <c r="G42" s="45">
-        <v>409</v>
+        <v>474</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="I42" s="21">
-        <v>42613</v>
+        <v>44562</v>
       </c>
       <c r="J42" s="21">
-        <v>45118</v>
+        <v>44910</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N42" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="L42" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="M42" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="N42" s="18"/>
       <c r="O42" s="4" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
       <c r="P42" s="4" t="s">
         <v>12</v>
@@ -4997,47 +4995,89 @@
         <v>23</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="T42" s="4" t="s">
         <v>205</v>
       </c>
       <c r="U42" s="4" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="V42" s="4"/>
+      <c r="W42" s="7"/>
+      <c r="X42" s="6"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <f>A42+1</f>
-        <v>42</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="45">
+        <v>47.4</v>
+      </c>
+      <c r="F43" s="45">
+        <v>8.5</v>
+      </c>
+      <c r="G43" s="45">
+        <v>409</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I43" s="21">
+        <v>42613</v>
+      </c>
+      <c r="J43" s="21">
+        <v>45118</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S43" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="T43" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="U43" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="V43" s="4"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <f>A43+1</f>
-        <v>43</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -5063,8 +5103,8 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <f>A44+1</f>
-        <v>44</v>
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5090,8 +5130,8 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <f>A45+1</f>
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -5117,8 +5157,8 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <f>A46+1</f>
-        <v>46</v>
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -5144,8 +5184,8 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <f>A47+1</f>
-        <v>47</v>
+        <f t="shared" si="1"/>
+        <v>46</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -5171,8 +5211,8 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <f>A48+1</f>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>47</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -5196,91 +5236,118 @@
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
     </row>
-    <row r="54" spans="1:22" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="20" t="s">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+    </row>
+    <row r="55" spans="1:22" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="20" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H55" s="57"/>
-      <c r="I55" s="24" t="s">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H56" s="57"/>
+      <c r="I56" s="24" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H56" s="59"/>
-      <c r="I56" s="24" t="s">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H57" s="59"/>
+      <c r="I57" s="24" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H57" s="60"/>
-      <c r="I57" s="24" t="s">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H58" s="60"/>
+      <c r="I58" s="24" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>33</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B61" s="16" t="s">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B62" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>180</v>
-      </c>
-      <c r="D62" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="D63" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>174</v>
+        <v>117</v>
       </c>
       <c r="D64" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>232</v>
+        <v>174</v>
       </c>
       <c r="D65" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
+        <v>232</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>295</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>294</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V49">
-    <sortCondition ref="C2:C49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V50">
+    <sortCondition ref="C2:C50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5291,7 +5358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAECC9E8-07B8-43E6-AF50-264301188E83}">
   <dimension ref="A2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -5606,10 +5673,10 @@
       <c r="H2" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="64"/>
+      <c r="J2" s="66"/>
       <c r="K2" s="14" t="s">
         <v>100</v>
       </c>

</xml_diff>